<commit_message>
add-to-cart 4 test cases added
</commit_message>
<xml_diff>
--- a/bin/testdata/trackTestdata.xlsx
+++ b/bin/testdata/trackTestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivam_kushwaha\eclipse-workspace\ShoppingPortal\src\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A4194D-EFAF-48F3-84C9-79DFE3CBB6D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEFAEA4-E9B7-4ED7-B85F-DD592D343563}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C5E69758-48B3-4D4F-90F2-E815ECD79B59}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>orderid</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>sk@g.com</t>
+  </si>
+  <si>
+    <t>sj@g.com</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Valid</t>
   </si>
 </sst>
 </file>
@@ -408,52 +420,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBC9619-9AFD-4ABE-8061-1935EE7A155B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1000</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1000</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>